<commit_message>
Update new CF for solar
</commit_message>
<xml_diff>
--- a/InputData/elec/BECF/BAU Expected Capacity Factors.xlsx
+++ b/InputData/elec/BECF/BAU Expected Capacity Factors.xlsx
@@ -5,7 +5,7 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-india\InputData\elec\BECF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganM\Documents\eps-india\InputData\elec\BECF\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
     <sheet name="BECF-pre-nonret" sheetId="5" r:id="rId8"/>
     <sheet name="BECF-new" sheetId="6" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1562,22 +1562,22 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2278,43 +2278,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
                 <c:pt idx="0">
-                  <c:v>0.19</c:v>
+                  <c:v>0.24</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.19384615384615422</c:v>
+                  <c:v>0.24</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.19769230769230806</c:v>
+                  <c:v>0.24</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.20153846153846189</c:v>
+                  <c:v>0.24</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.20538461538461572</c:v>
+                  <c:v>0.24</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.20923076923076955</c:v>
+                  <c:v>0.24</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.21307692307692339</c:v>
+                  <c:v>0.24</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.21692307692307722</c:v>
+                  <c:v>0.24</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.22076923076923105</c:v>
+                  <c:v>0.24</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.22461538461538488</c:v>
+                  <c:v>0.24</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.22846153846153872</c:v>
+                  <c:v>0.24</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.23230769230769255</c:v>
+                  <c:v>0.24</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.23615384615384638</c:v>
+                  <c:v>0.24</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0.24</c:v>
@@ -2642,6 +2642,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4769,27 +4770,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="36" t="s">
+      <c r="C2" s="39"/>
+      <c r="D2" s="37" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="38"/>
@@ -4798,52 +4799,52 @@
       <c r="H2" s="38"/>
       <c r="I2" s="38"/>
       <c r="J2" s="38"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="36" t="s">
+      <c r="K2" s="39"/>
+      <c r="L2" s="37" t="s">
         <v>5</v>
       </c>
       <c r="M2" s="38"/>
       <c r="N2" s="38"/>
       <c r="O2" s="38"/>
       <c r="P2" s="38"/>
-      <c r="Q2" s="37"/>
+      <c r="Q2" s="39"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A3" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="37"/>
-      <c r="D3" s="36" t="s">
+      <c r="C3" s="39"/>
+      <c r="D3" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="E3" s="37"/>
-      <c r="F3" s="36" t="s">
+      <c r="E3" s="39"/>
+      <c r="F3" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="G3" s="37"/>
-      <c r="H3" s="36" t="s">
+      <c r="G3" s="39"/>
+      <c r="H3" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="37"/>
-      <c r="J3" s="36" t="s">
+      <c r="I3" s="39"/>
+      <c r="J3" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="K3" s="37"/>
-      <c r="L3" s="36" t="s">
+      <c r="K3" s="39"/>
+      <c r="L3" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="M3" s="37"/>
-      <c r="N3" s="36" t="s">
+      <c r="M3" s="39"/>
+      <c r="N3" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="O3" s="37"/>
-      <c r="P3" s="36" t="s">
+      <c r="O3" s="39"/>
+      <c r="P3" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="Q3" s="37"/>
+      <c r="Q3" s="39"/>
     </row>
     <row r="4" spans="1:17" ht="39.75" x14ac:dyDescent="0.45">
       <c r="A4" s="9" t="s">
@@ -4899,25 +4900,25 @@
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="39"/>
-      <c r="J5" s="39"/>
-      <c r="K5" s="39"/>
-      <c r="L5" s="39"/>
-      <c r="M5" s="39"/>
-      <c r="N5" s="39"/>
-      <c r="O5" s="39"/>
-      <c r="P5" s="39"/>
-      <c r="Q5" s="39"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
+      <c r="L5" s="35"/>
+      <c r="M5" s="35"/>
+      <c r="N5" s="35"/>
+      <c r="O5" s="35"/>
+      <c r="P5" s="35"/>
+      <c r="Q5" s="35"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A6" s="12">
@@ -5450,25 +5451,25 @@
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A16" s="39" t="s">
+      <c r="A16" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="39"/>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="39"/>
-      <c r="G16" s="39"/>
-      <c r="H16" s="39"/>
-      <c r="I16" s="39"/>
-      <c r="J16" s="39"/>
-      <c r="K16" s="39"/>
-      <c r="L16" s="39"/>
-      <c r="M16" s="39"/>
-      <c r="N16" s="39"/>
-      <c r="O16" s="39"/>
-      <c r="P16" s="39"/>
-      <c r="Q16" s="39"/>
+      <c r="B16" s="35"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="35"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
+      <c r="K16" s="35"/>
+      <c r="L16" s="35"/>
+      <c r="M16" s="35"/>
+      <c r="N16" s="35"/>
+      <c r="O16" s="35"/>
+      <c r="P16" s="35"/>
+      <c r="Q16" s="35"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A17" s="12" t="s">
@@ -6107,25 +6108,25 @@
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="B29" s="39"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
-      <c r="K29" s="39"/>
-      <c r="L29" s="39"/>
-      <c r="M29" s="39"/>
-      <c r="N29" s="39"/>
-      <c r="O29" s="39"/>
-      <c r="P29" s="39"/>
-      <c r="Q29" s="39"/>
+      <c r="B29" s="35"/>
+      <c r="C29" s="35"/>
+      <c r="D29" s="35"/>
+      <c r="E29" s="35"/>
+      <c r="F29" s="35"/>
+      <c r="G29" s="35"/>
+      <c r="H29" s="35"/>
+      <c r="I29" s="35"/>
+      <c r="J29" s="35"/>
+      <c r="K29" s="35"/>
+      <c r="L29" s="35"/>
+      <c r="M29" s="35"/>
+      <c r="N29" s="35"/>
+      <c r="O29" s="35"/>
+      <c r="P29" s="35"/>
+      <c r="Q29" s="35"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A30" s="12" t="s">
@@ -6764,25 +6765,25 @@
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A42" s="39" t="s">
+      <c r="A42" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="B42" s="39"/>
-      <c r="C42" s="39"/>
-      <c r="D42" s="39"/>
-      <c r="E42" s="39"/>
-      <c r="F42" s="39"/>
-      <c r="G42" s="39"/>
-      <c r="H42" s="39"/>
-      <c r="I42" s="39"/>
-      <c r="J42" s="39"/>
-      <c r="K42" s="39"/>
-      <c r="L42" s="39"/>
-      <c r="M42" s="39"/>
-      <c r="N42" s="39"/>
-      <c r="O42" s="39"/>
-      <c r="P42" s="39"/>
-      <c r="Q42" s="39"/>
+      <c r="B42" s="35"/>
+      <c r="C42" s="35"/>
+      <c r="D42" s="35"/>
+      <c r="E42" s="35"/>
+      <c r="F42" s="35"/>
+      <c r="G42" s="35"/>
+      <c r="H42" s="35"/>
+      <c r="I42" s="35"/>
+      <c r="J42" s="35"/>
+      <c r="K42" s="35"/>
+      <c r="L42" s="35"/>
+      <c r="M42" s="35"/>
+      <c r="N42" s="35"/>
+      <c r="O42" s="35"/>
+      <c r="P42" s="35"/>
+      <c r="Q42" s="35"/>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A43" s="12" t="s">
@@ -7209,28 +7210,33 @@
       </c>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A51" s="40" t="s">
+      <c r="A51" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="B51" s="40"/>
-      <c r="C51" s="40"/>
-      <c r="D51" s="40"/>
-      <c r="E51" s="40"/>
-      <c r="F51" s="40"/>
-      <c r="G51" s="40"/>
-      <c r="H51" s="40"/>
-      <c r="I51" s="40"/>
-      <c r="J51" s="40"/>
-      <c r="K51" s="40"/>
-      <c r="L51" s="40"/>
-      <c r="M51" s="40"/>
-      <c r="N51" s="40"/>
-      <c r="O51" s="40"/>
-      <c r="P51" s="40"/>
-      <c r="Q51" s="40"/>
+      <c r="B51" s="36"/>
+      <c r="C51" s="36"/>
+      <c r="D51" s="36"/>
+      <c r="E51" s="36"/>
+      <c r="F51" s="36"/>
+      <c r="G51" s="36"/>
+      <c r="H51" s="36"/>
+      <c r="I51" s="36"/>
+      <c r="J51" s="36"/>
+      <c r="K51" s="36"/>
+      <c r="L51" s="36"/>
+      <c r="M51" s="36"/>
+      <c r="N51" s="36"/>
+      <c r="O51" s="36"/>
+      <c r="P51" s="36"/>
+      <c r="Q51" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:K2"/>
+    <mergeCell ref="A5:Q5"/>
+    <mergeCell ref="A16:Q16"/>
     <mergeCell ref="A42:Q42"/>
     <mergeCell ref="A51:Q51"/>
     <mergeCell ref="L2:Q2"/>
@@ -7243,11 +7249,6 @@
     <mergeCell ref="N3:O3"/>
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="A29:Q29"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:K2"/>
-    <mergeCell ref="A5:Q5"/>
-    <mergeCell ref="A16:Q16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7591,8 +7592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU34"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10:O10"/>
+    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22:AB22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7903,7 +7904,7 @@
         <v>24</v>
       </c>
       <c r="Q7" s="23">
-        <f t="shared" si="2"/>
+        <f>M7/100</f>
         <v>0.19</v>
       </c>
       <c r="R7" s="24">
@@ -9154,68 +9155,68 @@
         <v>21</v>
       </c>
       <c r="M22">
-        <f t="shared" si="5"/>
-        <v>0.19</v>
+        <f>$R$7</f>
+        <v>0.24</v>
       </c>
       <c r="N22">
-        <f>P22</f>
-        <v>0.19</v>
+        <f t="shared" ref="N22:AB22" si="17">$R$7</f>
+        <v>0.24</v>
       </c>
       <c r="O22">
-        <f>P22</f>
-        <v>0.19</v>
+        <f t="shared" si="17"/>
+        <v>0.24</v>
       </c>
       <c r="P22">
-        <f>Q7</f>
-        <v>0.19</v>
+        <f t="shared" si="17"/>
+        <v>0.24</v>
       </c>
       <c r="Q22">
-        <f>FORECAST(Q16,$Q$7:$R$7,$Q$2:$R$2)</f>
-        <v>0.19384615384615422</v>
+        <f t="shared" si="17"/>
+        <v>0.24</v>
       </c>
       <c r="R22">
-        <f t="shared" ref="R22:AB22" si="17">FORECAST(R16,$Q$7:$R$7,$Q$2:$R$2)</f>
-        <v>0.19769230769230806</v>
+        <f t="shared" si="17"/>
+        <v>0.24</v>
       </c>
       <c r="S22">
         <f t="shared" si="17"/>
-        <v>0.20153846153846189</v>
+        <v>0.24</v>
       </c>
       <c r="T22">
         <f t="shared" si="17"/>
-        <v>0.20538461538461572</v>
+        <v>0.24</v>
       </c>
       <c r="U22">
         <f t="shared" si="17"/>
-        <v>0.20923076923076955</v>
+        <v>0.24</v>
       </c>
       <c r="V22">
         <f t="shared" si="17"/>
-        <v>0.21307692307692339</v>
+        <v>0.24</v>
       </c>
       <c r="W22">
         <f t="shared" si="17"/>
-        <v>0.21692307692307722</v>
+        <v>0.24</v>
       </c>
       <c r="X22">
         <f t="shared" si="17"/>
-        <v>0.22076923076923105</v>
+        <v>0.24</v>
       </c>
       <c r="Y22">
         <f t="shared" si="17"/>
-        <v>0.22461538461538488</v>
+        <v>0.24</v>
       </c>
       <c r="Z22">
         <f t="shared" si="17"/>
-        <v>0.22846153846153872</v>
+        <v>0.24</v>
       </c>
       <c r="AA22">
         <f t="shared" si="17"/>
-        <v>0.23230769230769255</v>
+        <v>0.24</v>
       </c>
       <c r="AB22">
         <f t="shared" si="17"/>
-        <v>0.23615384615384638</v>
+        <v>0.24</v>
       </c>
       <c r="AC22">
         <f>R7</f>
@@ -15371,7 +15372,7 @@
   <dimension ref="A1:AL17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -16231,67 +16232,67 @@
       </c>
       <c r="B7" s="7">
         <f>Calculations!M22</f>
-        <v>0.19</v>
+        <v>0.24</v>
       </c>
       <c r="C7" s="7">
         <f>Calculations!N22</f>
-        <v>0.19</v>
+        <v>0.24</v>
       </c>
       <c r="D7" s="7">
         <f>Calculations!O22</f>
-        <v>0.19</v>
+        <v>0.24</v>
       </c>
       <c r="E7" s="7">
         <f>Calculations!P22</f>
-        <v>0.19</v>
+        <v>0.24</v>
       </c>
       <c r="F7" s="7">
         <f>Calculations!Q22</f>
-        <v>0.19384615384615422</v>
+        <v>0.24</v>
       </c>
       <c r="G7" s="7">
         <f>Calculations!R22</f>
-        <v>0.19769230769230806</v>
+        <v>0.24</v>
       </c>
       <c r="H7" s="7">
         <f>Calculations!S22</f>
-        <v>0.20153846153846189</v>
+        <v>0.24</v>
       </c>
       <c r="I7" s="7">
         <f>Calculations!T22</f>
-        <v>0.20538461538461572</v>
+        <v>0.24</v>
       </c>
       <c r="J7" s="7">
         <f>Calculations!U22</f>
-        <v>0.20923076923076955</v>
+        <v>0.24</v>
       </c>
       <c r="K7" s="7">
         <f>Calculations!V22</f>
-        <v>0.21307692307692339</v>
+        <v>0.24</v>
       </c>
       <c r="L7" s="7">
         <f>Calculations!W22</f>
-        <v>0.21692307692307722</v>
+        <v>0.24</v>
       </c>
       <c r="M7" s="7">
         <f>Calculations!X22</f>
-        <v>0.22076923076923105</v>
+        <v>0.24</v>
       </c>
       <c r="N7" s="7">
         <f>Calculations!Y22</f>
-        <v>0.22461538461538488</v>
+        <v>0.24</v>
       </c>
       <c r="O7" s="7">
         <f>Calculations!Z22</f>
-        <v>0.22846153846153872</v>
+        <v>0.24</v>
       </c>
       <c r="P7" s="7">
         <f>Calculations!AA22</f>
-        <v>0.23230769230769255</v>
+        <v>0.24</v>
       </c>
       <c r="Q7" s="7">
         <f>Calculations!AB22</f>
-        <v>0.23615384615384638</v>
+        <v>0.24</v>
       </c>
       <c r="R7" s="7">
         <f>Calculations!AC22</f>

</xml_diff>

<commit_message>
WRI edit to new solar BECF
</commit_message>
<xml_diff>
--- a/InputData/elec/BECF/BAU Expected Capacity Factors.xlsx
+++ b/InputData/elec/BECF/BAU Expected Capacity Factors.xlsx
@@ -22,7 +22,7 @@
     <sheet name="BECF-pre-nonret" sheetId="5" r:id="rId8"/>
     <sheet name="BECF-new" sheetId="6" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" iterate="1" iterateDelta="1.0000000000000001E-5"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -499,7 +499,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-SECI normative CUFs for sample tender - http://seci.co.in/web-data/docs/tenders/RfS_500%20MW%20Tamilnadu.pdf -- Sec 8.4a, pp 28</t>
+NREL/POSOCO table 6</t>
         </r>
       </text>
     </comment>
@@ -1562,22 +1562,22 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2278,46 +2278,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
                 <c:pt idx="0">
-                  <c:v>0.24</c:v>
+                  <c:v>0.21</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.24</c:v>
+                  <c:v>0.21230769230769209</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.24</c:v>
+                  <c:v>0.21461538461538421</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.24</c:v>
+                  <c:v>0.21692307692307722</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.24</c:v>
+                  <c:v>0.21923076923076934</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.24</c:v>
+                  <c:v>0.22153846153846146</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.24</c:v>
+                  <c:v>0.22384615384615358</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.24</c:v>
+                  <c:v>0.22615384615384571</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.24</c:v>
+                  <c:v>0.22846153846153872</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.24</c:v>
+                  <c:v>0.23076923076923084</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.24</c:v>
+                  <c:v>0.23307692307692296</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.24</c:v>
+                  <c:v>0.23538461538461508</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.24</c:v>
+                  <c:v>0.2376923076923072</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.24</c:v>
+                  <c:v>0.24000000000000021</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0.24</c:v>
@@ -3765,7 +3765,7 @@
   <dimension ref="A1:D66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4154,7 +4154,7 @@
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11:I11"/>
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4395,7 +4395,6 @@
         <v>74</v>
       </c>
       <c r="B8">
-        <f>Calculations!$M$7/100</f>
         <v>0.19</v>
       </c>
       <c r="C8">
@@ -4770,27 +4769,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="37" t="s">
+      <c r="C2" s="37"/>
+      <c r="D2" s="36" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="38"/>
@@ -4799,52 +4798,52 @@
       <c r="H2" s="38"/>
       <c r="I2" s="38"/>
       <c r="J2" s="38"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="37" t="s">
+      <c r="K2" s="37"/>
+      <c r="L2" s="36" t="s">
         <v>5</v>
       </c>
       <c r="M2" s="38"/>
       <c r="N2" s="38"/>
       <c r="O2" s="38"/>
       <c r="P2" s="38"/>
-      <c r="Q2" s="39"/>
+      <c r="Q2" s="37"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A3" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="39"/>
-      <c r="D3" s="37" t="s">
+      <c r="C3" s="37"/>
+      <c r="D3" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="E3" s="39"/>
-      <c r="F3" s="37" t="s">
+      <c r="E3" s="37"/>
+      <c r="F3" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="G3" s="39"/>
-      <c r="H3" s="37" t="s">
+      <c r="G3" s="37"/>
+      <c r="H3" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="39"/>
-      <c r="J3" s="37" t="s">
+      <c r="I3" s="37"/>
+      <c r="J3" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="K3" s="39"/>
-      <c r="L3" s="37" t="s">
+      <c r="K3" s="37"/>
+      <c r="L3" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="M3" s="39"/>
-      <c r="N3" s="37" t="s">
+      <c r="M3" s="37"/>
+      <c r="N3" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="O3" s="39"/>
-      <c r="P3" s="37" t="s">
+      <c r="O3" s="37"/>
+      <c r="P3" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="Q3" s="39"/>
+      <c r="Q3" s="37"/>
     </row>
     <row r="4" spans="1:17" ht="39.75" x14ac:dyDescent="0.45">
       <c r="A4" s="9" t="s">
@@ -4900,25 +4899,25 @@
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
-      <c r="I5" s="35"/>
-      <c r="J5" s="35"/>
-      <c r="K5" s="35"/>
-      <c r="L5" s="35"/>
-      <c r="M5" s="35"/>
-      <c r="N5" s="35"/>
-      <c r="O5" s="35"/>
-      <c r="P5" s="35"/>
-      <c r="Q5" s="35"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
+      <c r="J5" s="39"/>
+      <c r="K5" s="39"/>
+      <c r="L5" s="39"/>
+      <c r="M5" s="39"/>
+      <c r="N5" s="39"/>
+      <c r="O5" s="39"/>
+      <c r="P5" s="39"/>
+      <c r="Q5" s="39"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A6" s="12">
@@ -5451,25 +5450,25 @@
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="35"/>
-      <c r="C16" s="35"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="35"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
-      <c r="K16" s="35"/>
-      <c r="L16" s="35"/>
-      <c r="M16" s="35"/>
-      <c r="N16" s="35"/>
-      <c r="O16" s="35"/>
-      <c r="P16" s="35"/>
-      <c r="Q16" s="35"/>
+      <c r="B16" s="39"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="39"/>
+      <c r="G16" s="39"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="39"/>
+      <c r="J16" s="39"/>
+      <c r="K16" s="39"/>
+      <c r="L16" s="39"/>
+      <c r="M16" s="39"/>
+      <c r="N16" s="39"/>
+      <c r="O16" s="39"/>
+      <c r="P16" s="39"/>
+      <c r="Q16" s="39"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A17" s="12" t="s">
@@ -6108,25 +6107,25 @@
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A29" s="35" t="s">
+      <c r="A29" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="B29" s="35"/>
-      <c r="C29" s="35"/>
-      <c r="D29" s="35"/>
-      <c r="E29" s="35"/>
-      <c r="F29" s="35"/>
-      <c r="G29" s="35"/>
-      <c r="H29" s="35"/>
-      <c r="I29" s="35"/>
-      <c r="J29" s="35"/>
-      <c r="K29" s="35"/>
-      <c r="L29" s="35"/>
-      <c r="M29" s="35"/>
-      <c r="N29" s="35"/>
-      <c r="O29" s="35"/>
-      <c r="P29" s="35"/>
-      <c r="Q29" s="35"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
+      <c r="K29" s="39"/>
+      <c r="L29" s="39"/>
+      <c r="M29" s="39"/>
+      <c r="N29" s="39"/>
+      <c r="O29" s="39"/>
+      <c r="P29" s="39"/>
+      <c r="Q29" s="39"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A30" s="12" t="s">
@@ -6765,25 +6764,25 @@
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A42" s="35" t="s">
+      <c r="A42" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="B42" s="35"/>
-      <c r="C42" s="35"/>
-      <c r="D42" s="35"/>
-      <c r="E42" s="35"/>
-      <c r="F42" s="35"/>
-      <c r="G42" s="35"/>
-      <c r="H42" s="35"/>
-      <c r="I42" s="35"/>
-      <c r="J42" s="35"/>
-      <c r="K42" s="35"/>
-      <c r="L42" s="35"/>
-      <c r="M42" s="35"/>
-      <c r="N42" s="35"/>
-      <c r="O42" s="35"/>
-      <c r="P42" s="35"/>
-      <c r="Q42" s="35"/>
+      <c r="B42" s="39"/>
+      <c r="C42" s="39"/>
+      <c r="D42" s="39"/>
+      <c r="E42" s="39"/>
+      <c r="F42" s="39"/>
+      <c r="G42" s="39"/>
+      <c r="H42" s="39"/>
+      <c r="I42" s="39"/>
+      <c r="J42" s="39"/>
+      <c r="K42" s="39"/>
+      <c r="L42" s="39"/>
+      <c r="M42" s="39"/>
+      <c r="N42" s="39"/>
+      <c r="O42" s="39"/>
+      <c r="P42" s="39"/>
+      <c r="Q42" s="39"/>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A43" s="12" t="s">
@@ -7210,33 +7209,28 @@
       </c>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A51" s="36" t="s">
+      <c r="A51" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="B51" s="36"/>
-      <c r="C51" s="36"/>
-      <c r="D51" s="36"/>
-      <c r="E51" s="36"/>
-      <c r="F51" s="36"/>
-      <c r="G51" s="36"/>
-      <c r="H51" s="36"/>
-      <c r="I51" s="36"/>
-      <c r="J51" s="36"/>
-      <c r="K51" s="36"/>
-      <c r="L51" s="36"/>
-      <c r="M51" s="36"/>
-      <c r="N51" s="36"/>
-      <c r="O51" s="36"/>
-      <c r="P51" s="36"/>
-      <c r="Q51" s="36"/>
+      <c r="B51" s="40"/>
+      <c r="C51" s="40"/>
+      <c r="D51" s="40"/>
+      <c r="E51" s="40"/>
+      <c r="F51" s="40"/>
+      <c r="G51" s="40"/>
+      <c r="H51" s="40"/>
+      <c r="I51" s="40"/>
+      <c r="J51" s="40"/>
+      <c r="K51" s="40"/>
+      <c r="L51" s="40"/>
+      <c r="M51" s="40"/>
+      <c r="N51" s="40"/>
+      <c r="O51" s="40"/>
+      <c r="P51" s="40"/>
+      <c r="Q51" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:K2"/>
-    <mergeCell ref="A5:Q5"/>
-    <mergeCell ref="A16:Q16"/>
     <mergeCell ref="A42:Q42"/>
     <mergeCell ref="A51:Q51"/>
     <mergeCell ref="L2:Q2"/>
@@ -7249,6 +7243,11 @@
     <mergeCell ref="N3:O3"/>
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="A29:Q29"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:K2"/>
+    <mergeCell ref="A5:Q5"/>
+    <mergeCell ref="A16:Q16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7592,8 +7591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU34"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22:AB22"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AD22" sqref="AD22:AU22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7712,7 +7711,7 @@
         <v>57.43333333333328</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:C34" si="1">B4/100</f>
+        <f>B4/100</f>
         <v>0.57433333333333281</v>
       </c>
       <c r="D4">
@@ -7737,7 +7736,7 @@
         <v>40</v>
       </c>
       <c r="Q4" s="23">
-        <f t="shared" ref="Q4:Q14" si="2">M4/100</f>
+        <f>M4/100</f>
         <v>0.4</v>
       </c>
       <c r="R4" s="24">
@@ -7766,7 +7765,7 @@
     </row>
     <row r="5" spans="1:47" x14ac:dyDescent="0.45">
       <c r="A5">
-        <f t="shared" ref="A5:A34" si="3">A4+1</f>
+        <f>A4+1</f>
         <v>2021</v>
       </c>
       <c r="B5">
@@ -7774,7 +7773,7 @@
         <v>56.966666666666697</v>
       </c>
       <c r="C5">
-        <f t="shared" si="1"/>
+        <f>B5/100</f>
         <v>0.56966666666666699</v>
       </c>
       <c r="D5">
@@ -7799,7 +7798,7 @@
         <v>46.5</v>
       </c>
       <c r="Q5" s="23">
-        <f t="shared" si="2"/>
+        <f>M5/100</f>
         <v>0.375</v>
       </c>
       <c r="R5" s="24">
@@ -7822,7 +7821,7 @@
     </row>
     <row r="6" spans="1:47" x14ac:dyDescent="0.45">
       <c r="A6">
-        <f t="shared" si="3"/>
+        <f>A5+1</f>
         <v>2022</v>
       </c>
       <c r="B6">
@@ -7830,7 +7829,7 @@
         <v>56.5</v>
       </c>
       <c r="C6">
-        <f t="shared" si="1"/>
+        <f>B6/100</f>
         <v>0.56499999999999995</v>
       </c>
       <c r="D6">
@@ -7853,7 +7852,7 @@
         <v>44</v>
       </c>
       <c r="Q6" s="23">
-        <f t="shared" si="2"/>
+        <f>M6/100</f>
         <v>0.35499999999999998</v>
       </c>
       <c r="R6" s="24"/>
@@ -7872,7 +7871,7 @@
     </row>
     <row r="7" spans="1:47" x14ac:dyDescent="0.45">
       <c r="A7">
-        <f t="shared" si="3"/>
+        <f>A6+1</f>
         <v>2023</v>
       </c>
       <c r="B7">
@@ -7880,7 +7879,7 @@
         <v>57.299999999999955</v>
       </c>
       <c r="C7">
-        <f t="shared" si="1"/>
+        <f>B7/100</f>
         <v>0.57299999999999951</v>
       </c>
       <c r="D7">
@@ -7893,7 +7892,7 @@
         <v>74</v>
       </c>
       <c r="M7">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="N7">
         <f>'IESS+others'!F8*100</f>
@@ -7905,7 +7904,7 @@
       </c>
       <c r="Q7" s="23">
         <f>M7/100</f>
-        <v>0.19</v>
+        <v>0.21</v>
       </c>
       <c r="R7" s="24">
         <f t="shared" si="0"/>
@@ -7918,7 +7917,7 @@
     </row>
     <row r="8" spans="1:47" x14ac:dyDescent="0.45">
       <c r="A8">
-        <f t="shared" si="3"/>
+        <f>A7+1</f>
         <v>2024</v>
       </c>
       <c r="B8">
@@ -7926,7 +7925,7 @@
         <v>58.099999999999909</v>
       </c>
       <c r="C8">
-        <f t="shared" si="1"/>
+        <f>B8/100</f>
         <v>0.58099999999999907</v>
       </c>
       <c r="D8">
@@ -7950,7 +7949,7 @@
         <v>46</v>
       </c>
       <c r="Q8" s="23">
-        <f t="shared" si="2"/>
+        <f>M8/100</f>
         <v>0.28749999999999998</v>
       </c>
       <c r="R8" s="24">
@@ -7964,7 +7963,7 @@
     </row>
     <row r="9" spans="1:47" x14ac:dyDescent="0.45">
       <c r="A9">
-        <f t="shared" si="3"/>
+        <f>A8+1</f>
         <v>2025</v>
       </c>
       <c r="B9">
@@ -7972,7 +7971,7 @@
         <v>58.899999999999864</v>
       </c>
       <c r="C9">
-        <f t="shared" si="1"/>
+        <f>B9/100</f>
         <v>0.58899999999999864</v>
       </c>
       <c r="D9">
@@ -7996,7 +7995,7 @@
         <v>30</v>
       </c>
       <c r="Q9" s="23">
-        <f t="shared" si="2"/>
+        <f>M9/100</f>
         <v>0.3</v>
       </c>
       <c r="R9" s="24">
@@ -8010,7 +8009,7 @@
     </row>
     <row r="10" spans="1:47" x14ac:dyDescent="0.45">
       <c r="A10">
-        <f t="shared" si="3"/>
+        <f>A9+1</f>
         <v>2026</v>
       </c>
       <c r="B10">
@@ -8018,7 +8017,7 @@
         <v>59.700000000000045</v>
       </c>
       <c r="C10">
-        <f t="shared" si="1"/>
+        <f>B10/100</f>
         <v>0.59700000000000042</v>
       </c>
       <c r="D10">
@@ -8043,7 +8042,7 @@
         <v>22.689835106537267</v>
       </c>
       <c r="Q10" s="23">
-        <f t="shared" si="2"/>
+        <f>M10/100</f>
         <v>0.22689835106537268</v>
       </c>
       <c r="R10" s="24">
@@ -8057,7 +8056,7 @@
     </row>
     <row r="11" spans="1:47" x14ac:dyDescent="0.45">
       <c r="A11">
-        <f t="shared" si="3"/>
+        <f>A10+1</f>
         <v>2027</v>
       </c>
       <c r="B11">
@@ -8065,7 +8064,7 @@
         <v>60.5</v>
       </c>
       <c r="C11">
-        <f t="shared" si="1"/>
+        <f>B11/100</f>
         <v>0.60499999999999998</v>
       </c>
       <c r="L11" t="s">
@@ -8084,7 +8083,7 @@
         <v>39</v>
       </c>
       <c r="Q11" s="23">
-        <f t="shared" si="2"/>
+        <f>M11/100</f>
         <v>0.36</v>
       </c>
       <c r="R11" s="24">
@@ -8098,7 +8097,7 @@
     </row>
     <row r="12" spans="1:47" x14ac:dyDescent="0.45">
       <c r="A12">
-        <f t="shared" si="3"/>
+        <f>A11+1</f>
         <v>2028</v>
       </c>
       <c r="B12">
@@ -8106,7 +8105,7 @@
         <v>63.399999999999636</v>
       </c>
       <c r="C12">
-        <f t="shared" si="1"/>
+        <f>B12/100</f>
         <v>0.63399999999999634</v>
       </c>
       <c r="L12" t="s">
@@ -8125,7 +8124,7 @@
         <v>76</v>
       </c>
       <c r="Q12" s="23">
-        <f t="shared" si="2"/>
+        <f>M12/100</f>
         <v>0.57899999999999996</v>
       </c>
       <c r="R12" s="24">
@@ -8139,7 +8138,7 @@
     </row>
     <row r="13" spans="1:47" x14ac:dyDescent="0.45">
       <c r="A13">
-        <f t="shared" si="3"/>
+        <f>A12+1</f>
         <v>2029</v>
       </c>
       <c r="B13">
@@ -8147,7 +8146,7 @@
         <v>66.299999999999272</v>
       </c>
       <c r="C13">
-        <f t="shared" si="1"/>
+        <f>B13/100</f>
         <v>0.66299999999999271</v>
       </c>
       <c r="L13" t="s">
@@ -8166,7 +8165,7 @@
         <v>45</v>
       </c>
       <c r="Q13" s="23">
-        <f t="shared" si="2"/>
+        <f>M13/100</f>
         <v>0.23309999999999997</v>
       </c>
       <c r="R13" s="24">
@@ -8180,7 +8179,7 @@
     </row>
     <row r="14" spans="1:47" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A14">
-        <f t="shared" si="3"/>
+        <f>A13+1</f>
         <v>2030</v>
       </c>
       <c r="B14">
@@ -8188,7 +8187,7 @@
         <v>69.199999999999818</v>
       </c>
       <c r="C14">
-        <f t="shared" si="1"/>
+        <f>B14/100</f>
         <v>0.69199999999999817</v>
       </c>
       <c r="L14" t="s">
@@ -8207,7 +8206,7 @@
         <v>76</v>
       </c>
       <c r="Q14" s="26">
-        <f t="shared" si="2"/>
+        <f>M14/100</f>
         <v>0.56950000000000001</v>
       </c>
       <c r="R14" s="27">
@@ -8221,7 +8220,7 @@
     </row>
     <row r="15" spans="1:47" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A15">
-        <f t="shared" si="3"/>
+        <f>A14+1</f>
         <v>2031</v>
       </c>
       <c r="B15">
@@ -8229,13 +8228,13 @@
         <v>72.099999999999454</v>
       </c>
       <c r="C15">
-        <f t="shared" si="1"/>
+        <f>B15/100</f>
         <v>0.72099999999999453</v>
       </c>
     </row>
     <row r="16" spans="1:47" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A16">
-        <f t="shared" si="3"/>
+        <f>A15+1</f>
         <v>2032</v>
       </c>
       <c r="B16">
@@ -8243,7 +8242,7 @@
         <v>75</v>
       </c>
       <c r="C16">
-        <f t="shared" si="1"/>
+        <f>B16/100</f>
         <v>0.75</v>
       </c>
       <c r="L16" s="30" t="s">
@@ -8265,129 +8264,129 @@
         <v>2020</v>
       </c>
       <c r="R16">
-        <f t="shared" ref="R16:AU16" si="4">Q16+1</f>
+        <f t="shared" ref="R16:AU16" si="1">Q16+1</f>
         <v>2021</v>
       </c>
       <c r="S16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>2022</v>
       </c>
       <c r="T16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>2023</v>
       </c>
       <c r="U16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>2024</v>
       </c>
       <c r="V16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>2025</v>
       </c>
       <c r="W16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>2026</v>
       </c>
       <c r="X16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>2027</v>
       </c>
       <c r="Y16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>2028</v>
       </c>
       <c r="Z16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>2029</v>
       </c>
       <c r="AA16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>2030</v>
       </c>
       <c r="AB16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>2031</v>
       </c>
       <c r="AC16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>2032</v>
       </c>
       <c r="AD16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>2033</v>
       </c>
       <c r="AE16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>2034</v>
       </c>
       <c r="AF16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>2035</v>
       </c>
       <c r="AG16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>2036</v>
       </c>
       <c r="AH16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>2037</v>
       </c>
       <c r="AI16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>2038</v>
       </c>
       <c r="AJ16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>2039</v>
       </c>
       <c r="AK16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>2040</v>
       </c>
       <c r="AL16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>2041</v>
       </c>
       <c r="AM16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>2042</v>
       </c>
       <c r="AN16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>2043</v>
       </c>
       <c r="AO16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>2044</v>
       </c>
       <c r="AP16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>2045</v>
       </c>
       <c r="AQ16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>2046</v>
       </c>
       <c r="AR16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>2047</v>
       </c>
       <c r="AS16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>2048</v>
       </c>
       <c r="AT16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>2049</v>
       </c>
       <c r="AU16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>2050</v>
       </c>
     </row>
     <row r="17" spans="1:47" x14ac:dyDescent="0.45">
       <c r="A17">
-        <f t="shared" si="3"/>
+        <f>A16+1</f>
         <v>2033</v>
       </c>
       <c r="B17">
@@ -8395,14 +8394,14 @@
         <v>75.199999999999989</v>
       </c>
       <c r="C17">
-        <f t="shared" si="1"/>
+        <f>B17/100</f>
         <v>0.75199999999999989</v>
       </c>
       <c r="L17" t="s">
         <v>34</v>
       </c>
       <c r="M17">
-        <f t="shared" ref="M17:M24" si="5">P17</f>
+        <f t="shared" ref="M17:M24" si="2">P17</f>
         <v>0.57899999999999996</v>
       </c>
       <c r="N17">
@@ -8512,7 +8511,7 @@
     </row>
     <row r="18" spans="1:47" x14ac:dyDescent="0.45">
       <c r="A18">
-        <f t="shared" si="3"/>
+        <f>A17+1</f>
         <v>2034</v>
       </c>
       <c r="B18">
@@ -8520,14 +8519,14 @@
         <v>75.399999999999977</v>
       </c>
       <c r="C18">
-        <f t="shared" si="1"/>
+        <f>B18/100</f>
         <v>0.75399999999999978</v>
       </c>
       <c r="L18" t="s">
         <v>18</v>
       </c>
       <c r="M18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>0.23309999999999997</v>
       </c>
       <c r="N18">
@@ -8547,47 +8546,47 @@
         <v>0.24978461538461261</v>
       </c>
       <c r="R18">
-        <f t="shared" ref="R18:AB18" si="6">FORECAST(R16,$Q$13:$R$13,$Q$2:$R$2)</f>
+        <f t="shared" ref="R18:AB18" si="3">FORECAST(R16,$Q$13:$R$13,$Q$2:$R$2)</f>
         <v>0.26646923076922491</v>
       </c>
       <c r="S18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>0.28315384615384431</v>
       </c>
       <c r="T18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>0.29983846153845661</v>
       </c>
       <c r="U18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>0.31652307692307602</v>
       </c>
       <c r="V18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>0.33320769230768832</v>
       </c>
       <c r="W18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>0.34989230769230062</v>
       </c>
       <c r="X18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>0.36657692307692002</v>
       </c>
       <c r="Y18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>0.38326153846153233</v>
       </c>
       <c r="Z18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>0.39994615384615173</v>
       </c>
       <c r="AA18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>0.41663076923076403</v>
       </c>
       <c r="AB18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>0.43331538461538344</v>
       </c>
       <c r="AC18">
@@ -8599,55 +8598,55 @@
         <v>0.45</v>
       </c>
       <c r="AE18">
-        <f t="shared" ref="AE18:AU18" si="7">AD18</f>
+        <f t="shared" ref="AE18:AU18" si="4">AD18</f>
         <v>0.45</v>
       </c>
       <c r="AF18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>0.45</v>
       </c>
       <c r="AG18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>0.45</v>
       </c>
       <c r="AH18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>0.45</v>
       </c>
       <c r="AI18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>0.45</v>
       </c>
       <c r="AJ18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>0.45</v>
       </c>
       <c r="AK18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>0.45</v>
       </c>
       <c r="AL18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>0.45</v>
       </c>
       <c r="AM18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>0.45</v>
       </c>
       <c r="AN18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>0.45</v>
       </c>
       <c r="AO18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>0.45</v>
       </c>
       <c r="AP18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>0.45</v>
       </c>
       <c r="AQ18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>0.45</v>
       </c>
       <c r="AR18">
@@ -8655,21 +8654,21 @@
         <v>0.45</v>
       </c>
       <c r="AS18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>0.45</v>
       </c>
       <c r="AT18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>0.45</v>
       </c>
       <c r="AU18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="4"/>
         <v>0.45</v>
       </c>
     </row>
     <row r="19" spans="1:47" x14ac:dyDescent="0.45">
       <c r="A19">
-        <f t="shared" si="3"/>
+        <f>A18+1</f>
         <v>2035</v>
       </c>
       <c r="B19">
@@ -8677,14 +8676,14 @@
         <v>75.599999999999966</v>
       </c>
       <c r="C19">
-        <f t="shared" si="1"/>
+        <f>B19/100</f>
         <v>0.75599999999999967</v>
       </c>
       <c r="L19" t="s">
         <v>19</v>
       </c>
       <c r="M19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>0.64599999999999991</v>
       </c>
       <c r="N19">
@@ -8704,47 +8703,47 @@
         <v>0.65784615384615464</v>
       </c>
       <c r="R19">
-        <f t="shared" ref="R19:AB19" si="8">FORECAST(R16,$Q$3:$R$3,$Q$2:$R$2)</f>
+        <f t="shared" ref="R19:AB19" si="5">FORECAST(R16,$Q$3:$R$3,$Q$2:$R$2)</f>
         <v>0.66969230769230847</v>
       </c>
       <c r="S19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>0.68153846153846231</v>
       </c>
       <c r="T19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>0.69338461538461615</v>
       </c>
       <c r="U19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>0.70523076923076999</v>
       </c>
       <c r="V19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>0.71707692307692383</v>
       </c>
       <c r="W19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>0.72892307692307767</v>
       </c>
       <c r="X19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>0.74076923076923151</v>
       </c>
       <c r="Y19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>0.75261538461538535</v>
       </c>
       <c r="Z19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>0.76446153846153919</v>
       </c>
       <c r="AA19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>0.77630769230769303</v>
       </c>
       <c r="AB19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="5"/>
         <v>0.78815384615384687</v>
       </c>
       <c r="AC19">
@@ -8756,55 +8755,55 @@
         <v>0.8</v>
       </c>
       <c r="AE19">
-        <f t="shared" ref="AE19:AQ19" si="9">AD19</f>
+        <f t="shared" ref="AE19:AQ19" si="6">AD19</f>
         <v>0.8</v>
       </c>
       <c r="AF19">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>0.8</v>
       </c>
       <c r="AG19">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>0.8</v>
       </c>
       <c r="AH19">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>0.8</v>
       </c>
       <c r="AI19">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>0.8</v>
       </c>
       <c r="AJ19">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>0.8</v>
       </c>
       <c r="AK19">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>0.8</v>
       </c>
       <c r="AL19">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>0.8</v>
       </c>
       <c r="AM19">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>0.8</v>
       </c>
       <c r="AN19">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>0.8</v>
       </c>
       <c r="AO19">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>0.8</v>
       </c>
       <c r="AP19">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>0.8</v>
       </c>
       <c r="AQ19">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>0.8</v>
       </c>
       <c r="AR19">
@@ -8816,17 +8815,17 @@
         <v>0.8</v>
       </c>
       <c r="AT19">
-        <f t="shared" ref="AT19:AU19" si="10">AS19</f>
+        <f t="shared" ref="AT19:AU19" si="7">AS19</f>
         <v>0.8</v>
       </c>
       <c r="AU19">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>0.8</v>
       </c>
     </row>
     <row r="20" spans="1:47" x14ac:dyDescent="0.45">
       <c r="A20">
-        <f t="shared" si="3"/>
+        <f>A19+1</f>
         <v>2036</v>
       </c>
       <c r="B20">
@@ -8834,14 +8833,14 @@
         <v>75.800000000000011</v>
       </c>
       <c r="C20">
-        <f t="shared" si="1"/>
+        <f>B20/100</f>
         <v>0.75800000000000012</v>
       </c>
       <c r="L20" t="s">
         <v>20</v>
       </c>
       <c r="M20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>0.39750000000000008</v>
       </c>
       <c r="N20">
@@ -8861,47 +8860,47 @@
         <v>0.39803846153846156</v>
       </c>
       <c r="R20">
-        <f t="shared" ref="R20:AB20" si="11">FORECAST(R16,$T$4:$U$4,$Q$2:$R$2)</f>
+        <f t="shared" ref="R20:AB20" si="8">FORECAST(R16,$T$4:$U$4,$Q$2:$R$2)</f>
         <v>0.39857692307692316</v>
       </c>
       <c r="S20">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>0.39911538461538476</v>
       </c>
       <c r="T20">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>0.39965384615384614</v>
       </c>
       <c r="U20">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>0.40019230769230774</v>
       </c>
       <c r="V20">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>0.40073076923076933</v>
       </c>
       <c r="W20">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>0.40126923076923071</v>
       </c>
       <c r="X20">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>0.40180769230769231</v>
       </c>
       <c r="Y20">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>0.40234615384615391</v>
       </c>
       <c r="Z20">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>0.40288461538461529</v>
       </c>
       <c r="AA20">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>0.40342307692307688</v>
       </c>
       <c r="AB20">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>0.40396153846153848</v>
       </c>
       <c r="AC20">
@@ -8913,55 +8912,55 @@
         <v>0.40463333333333334</v>
       </c>
       <c r="AE20">
-        <f t="shared" ref="AE20:AQ20" si="12">FORECAST(AE16,$U$4:$V$4,$R$2:$S$2)</f>
+        <f t="shared" ref="AE20:AQ20" si="9">FORECAST(AE16,$U$4:$V$4,$R$2:$S$2)</f>
         <v>0.40476666666666666</v>
       </c>
       <c r="AF20">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>0.40490000000000004</v>
       </c>
       <c r="AG20">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>0.40503333333333336</v>
       </c>
       <c r="AH20">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>0.40516666666666667</v>
       </c>
       <c r="AI20">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>0.40529999999999999</v>
       </c>
       <c r="AJ20">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>0.40543333333333337</v>
       </c>
       <c r="AK20">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>0.40556666666666669</v>
       </c>
       <c r="AL20">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>0.40570000000000001</v>
       </c>
       <c r="AM20">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>0.40583333333333332</v>
       </c>
       <c r="AN20">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>0.4059666666666667</v>
       </c>
       <c r="AO20">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>0.40610000000000002</v>
       </c>
       <c r="AP20">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>0.40623333333333334</v>
       </c>
       <c r="AQ20">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>0.40636666666666665</v>
       </c>
       <c r="AR20">
@@ -8973,17 +8972,17 @@
         <v>0.40650000000000003</v>
       </c>
       <c r="AT20">
-        <f t="shared" ref="AT20:AU20" si="13">AS20</f>
+        <f t="shared" ref="AT20:AU20" si="10">AS20</f>
         <v>0.40650000000000003</v>
       </c>
       <c r="AU20">
-        <f t="shared" si="13"/>
+        <f t="shared" si="10"/>
         <v>0.40650000000000003</v>
       </c>
     </row>
     <row r="21" spans="1:47" x14ac:dyDescent="0.45">
       <c r="A21">
-        <f t="shared" si="3"/>
+        <f>A20+1</f>
         <v>2037</v>
       </c>
       <c r="B21">
@@ -8991,14 +8990,14 @@
         <v>76</v>
       </c>
       <c r="C21">
-        <f t="shared" si="1"/>
+        <f>B21/100</f>
         <v>0.76</v>
       </c>
       <c r="L21" t="s">
         <v>33</v>
       </c>
       <c r="M21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>0.35499999999999998</v>
       </c>
       <c r="N21">
@@ -9018,107 +9017,107 @@
         <v>0.35803571428571423</v>
       </c>
       <c r="R21">
-        <f t="shared" ref="R21:AQ21" si="14">FORECAST(R16,$T$6:$U$6,$T$5:$U$5)</f>
+        <f t="shared" ref="R21:AQ21" si="11">FORECAST(R16,$T$6:$U$6,$T$5:$U$5)</f>
         <v>0.36107142857142804</v>
       </c>
       <c r="S21">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>0.36410714285714274</v>
       </c>
       <c r="T21">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>0.36714285714285744</v>
       </c>
       <c r="U21">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>0.37017857142857125</v>
       </c>
       <c r="V21">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>0.37321428571428594</v>
       </c>
       <c r="W21">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>0.37624999999999975</v>
       </c>
       <c r="X21">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>0.37928571428571445</v>
       </c>
       <c r="Y21">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>0.38232142857142826</v>
       </c>
       <c r="Z21">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>0.38535714285714295</v>
       </c>
       <c r="AA21">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>0.38839285714285676</v>
       </c>
       <c r="AB21">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>0.39142857142857146</v>
       </c>
       <c r="AC21">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>0.39446428571428527</v>
       </c>
       <c r="AD21">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>0.39749999999999996</v>
       </c>
       <c r="AE21">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>0.40053571428571377</v>
       </c>
       <c r="AF21">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>0.40357142857142847</v>
       </c>
       <c r="AG21">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>0.40660714285714317</v>
       </c>
       <c r="AH21">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>0.40964285714285698</v>
       </c>
       <c r="AI21">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>0.41267857142857167</v>
       </c>
       <c r="AJ21">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>0.41571428571428548</v>
       </c>
       <c r="AK21">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>0.41875000000000018</v>
       </c>
       <c r="AL21">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>0.42178571428571399</v>
       </c>
       <c r="AM21">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>0.42482142857142868</v>
       </c>
       <c r="AN21">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>0.42785714285714249</v>
       </c>
       <c r="AO21">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>0.43089285714285719</v>
       </c>
       <c r="AP21">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>0.433928571428571</v>
       </c>
       <c r="AQ21">
-        <f t="shared" si="14"/>
+        <f t="shared" si="11"/>
         <v>0.43696428571428569</v>
       </c>
       <c r="AR21">
@@ -9130,189 +9129,189 @@
         <v>0.44</v>
       </c>
       <c r="AT21">
-        <f t="shared" ref="AT21:AU23" si="15">AS21</f>
+        <f t="shared" ref="AT21:AU23" si="12">AS21</f>
         <v>0.44</v>
       </c>
       <c r="AU21">
-        <f t="shared" si="15"/>
+        <f t="shared" si="12"/>
         <v>0.44</v>
       </c>
     </row>
     <row r="22" spans="1:47" x14ac:dyDescent="0.45">
       <c r="A22">
-        <f t="shared" si="3"/>
+        <f>A21+1</f>
         <v>2038</v>
       </c>
       <c r="B22">
-        <f t="shared" ref="B22:B34" si="16">$B$21</f>
+        <f t="shared" ref="B22:B34" si="13">$B$21</f>
         <v>76</v>
       </c>
       <c r="C22">
-        <f t="shared" si="1"/>
+        <f>B22/100</f>
         <v>0.76</v>
       </c>
       <c r="L22" t="s">
         <v>21</v>
       </c>
       <c r="M22">
-        <f>$R$7</f>
+        <f>$P$22</f>
+        <v>0.21</v>
+      </c>
+      <c r="N22">
+        <f t="shared" ref="N22:O22" si="14">$P$22</f>
+        <v>0.21</v>
+      </c>
+      <c r="O22">
+        <f t="shared" si="14"/>
+        <v>0.21</v>
+      </c>
+      <c r="P22">
+        <f>Q7</f>
+        <v>0.21</v>
+      </c>
+      <c r="Q22">
+        <f>TREND($Q$7:$R$7,$Q$2:$R$2,Q16)</f>
+        <v>0.21230769230769209</v>
+      </c>
+      <c r="R22">
+        <f t="shared" ref="R22:AD22" si="15">TREND($Q$7:$R$7,$Q$2:$R$2,R16)</f>
+        <v>0.21461538461538421</v>
+      </c>
+      <c r="S22">
+        <f t="shared" si="15"/>
+        <v>0.21692307692307722</v>
+      </c>
+      <c r="T22">
+        <f t="shared" si="15"/>
+        <v>0.21923076923076934</v>
+      </c>
+      <c r="U22">
+        <f t="shared" si="15"/>
+        <v>0.22153846153846146</v>
+      </c>
+      <c r="V22">
+        <f t="shared" si="15"/>
+        <v>0.22384615384615358</v>
+      </c>
+      <c r="W22">
+        <f t="shared" si="15"/>
+        <v>0.22615384615384571</v>
+      </c>
+      <c r="X22">
+        <f t="shared" si="15"/>
+        <v>0.22846153846153872</v>
+      </c>
+      <c r="Y22">
+        <f t="shared" si="15"/>
+        <v>0.23076923076923084</v>
+      </c>
+      <c r="Z22">
+        <f t="shared" si="15"/>
+        <v>0.23307692307692296</v>
+      </c>
+      <c r="AA22">
+        <f t="shared" si="15"/>
+        <v>0.23538461538461508</v>
+      </c>
+      <c r="AB22">
+        <f t="shared" si="15"/>
+        <v>0.2376923076923072</v>
+      </c>
+      <c r="AC22">
+        <f t="shared" si="15"/>
+        <v>0.24000000000000021</v>
+      </c>
+      <c r="AD22">
+        <f>TREND($R$7:$S$7,$R$2:$S$2,AD16)</f>
         <v>0.24</v>
       </c>
-      <c r="N22">
-        <f t="shared" ref="N22:AB22" si="17">$R$7</f>
+      <c r="AE22">
+        <f t="shared" ref="AE22:AU22" si="16">TREND($R$7:$S$7,$R$2:$S$2,AE16)</f>
         <v>0.24</v>
       </c>
-      <c r="O22">
-        <f t="shared" si="17"/>
+      <c r="AF22">
+        <f t="shared" si="16"/>
         <v>0.24</v>
       </c>
-      <c r="P22">
-        <f t="shared" si="17"/>
+      <c r="AG22">
+        <f t="shared" si="16"/>
         <v>0.24</v>
       </c>
-      <c r="Q22">
-        <f t="shared" si="17"/>
+      <c r="AH22">
+        <f t="shared" si="16"/>
         <v>0.24</v>
       </c>
-      <c r="R22">
-        <f t="shared" si="17"/>
+      <c r="AI22">
+        <f t="shared" si="16"/>
         <v>0.24</v>
       </c>
-      <c r="S22">
-        <f t="shared" si="17"/>
+      <c r="AJ22">
+        <f t="shared" si="16"/>
         <v>0.24</v>
       </c>
-      <c r="T22">
-        <f t="shared" si="17"/>
+      <c r="AK22">
+        <f t="shared" si="16"/>
         <v>0.24</v>
       </c>
-      <c r="U22">
-        <f t="shared" si="17"/>
+      <c r="AL22">
+        <f t="shared" si="16"/>
         <v>0.24</v>
       </c>
-      <c r="V22">
-        <f t="shared" si="17"/>
+      <c r="AM22">
+        <f t="shared" si="16"/>
         <v>0.24</v>
       </c>
-      <c r="W22">
-        <f t="shared" si="17"/>
+      <c r="AN22">
+        <f t="shared" si="16"/>
         <v>0.24</v>
       </c>
-      <c r="X22">
-        <f t="shared" si="17"/>
+      <c r="AO22">
+        <f t="shared" si="16"/>
         <v>0.24</v>
       </c>
-      <c r="Y22">
-        <f t="shared" si="17"/>
+      <c r="AP22">
+        <f t="shared" si="16"/>
         <v>0.24</v>
       </c>
-      <c r="Z22">
-        <f t="shared" si="17"/>
+      <c r="AQ22">
+        <f t="shared" si="16"/>
         <v>0.24</v>
       </c>
-      <c r="AA22">
-        <f t="shared" si="17"/>
+      <c r="AR22">
+        <f t="shared" si="16"/>
         <v>0.24</v>
       </c>
-      <c r="AB22">
-        <f t="shared" si="17"/>
+      <c r="AS22">
+        <f t="shared" si="16"/>
         <v>0.24</v>
       </c>
-      <c r="AC22">
-        <f>R7</f>
+      <c r="AT22">
+        <f t="shared" si="16"/>
         <v>0.24</v>
       </c>
-      <c r="AD22">
-        <f>AC22</f>
-        <v>0.24</v>
-      </c>
-      <c r="AE22">
-        <f t="shared" ref="AE22:AQ22" si="18">AD22</f>
-        <v>0.24</v>
-      </c>
-      <c r="AF22">
-        <f t="shared" si="18"/>
-        <v>0.24</v>
-      </c>
-      <c r="AG22">
-        <f t="shared" si="18"/>
-        <v>0.24</v>
-      </c>
-      <c r="AH22">
-        <f t="shared" si="18"/>
-        <v>0.24</v>
-      </c>
-      <c r="AI22">
-        <f t="shared" si="18"/>
-        <v>0.24</v>
-      </c>
-      <c r="AJ22">
-        <f t="shared" si="18"/>
-        <v>0.24</v>
-      </c>
-      <c r="AK22">
-        <f t="shared" si="18"/>
-        <v>0.24</v>
-      </c>
-      <c r="AL22">
-        <f t="shared" si="18"/>
-        <v>0.24</v>
-      </c>
-      <c r="AM22">
-        <f t="shared" si="18"/>
-        <v>0.24</v>
-      </c>
-      <c r="AN22">
-        <f t="shared" si="18"/>
-        <v>0.24</v>
-      </c>
-      <c r="AO22">
-        <f t="shared" si="18"/>
-        <v>0.24</v>
-      </c>
-      <c r="AP22">
-        <f t="shared" si="18"/>
-        <v>0.24</v>
-      </c>
-      <c r="AQ22">
-        <f t="shared" si="18"/>
-        <v>0.24</v>
-      </c>
-      <c r="AR22">
-        <f>S7</f>
-        <v>0.24</v>
-      </c>
-      <c r="AS22">
-        <f>AR22</f>
-        <v>0.24</v>
-      </c>
-      <c r="AT22">
-        <f t="shared" si="15"/>
-        <v>0.24</v>
-      </c>
       <c r="AU22">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.24</v>
       </c>
     </row>
     <row r="23" spans="1:47" x14ac:dyDescent="0.45">
       <c r="A23">
-        <f t="shared" si="3"/>
+        <f>A22+1</f>
         <v>2039</v>
       </c>
       <c r="B23">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v>76</v>
       </c>
       <c r="C23">
-        <f t="shared" si="1"/>
+        <f>B23/100</f>
         <v>0.76</v>
       </c>
       <c r="L23" t="s">
         <v>22</v>
       </c>
       <c r="M23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>0.28749999999999998</v>
       </c>
       <c r="N23">
@@ -9332,47 +9331,47 @@
         <v>0.30076923076923379</v>
       </c>
       <c r="R23">
-        <f t="shared" ref="R23:AB23" si="19">FORECAST(R16,$Q$8:$R$8,$Q$2:$R$2)</f>
+        <f t="shared" ref="R23:AB23" si="17">FORECAST(R16,$Q$8:$R$8,$Q$2:$R$2)</f>
         <v>0.3140384615384626</v>
       </c>
       <c r="S23">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>0.32730769230769496</v>
       </c>
       <c r="T23">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>0.34057692307692378</v>
       </c>
       <c r="U23">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>0.35384615384615614</v>
       </c>
       <c r="V23">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>0.36711538461538495</v>
       </c>
       <c r="W23">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>0.38038461538461732</v>
       </c>
       <c r="X23">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>0.39365384615384613</v>
       </c>
       <c r="Y23">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>0.4069230769230785</v>
       </c>
       <c r="Z23">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>0.42019230769231086</v>
       </c>
       <c r="AA23">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>0.43346153846153967</v>
       </c>
       <c r="AB23">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>0.44673076923077204</v>
       </c>
       <c r="AC23">
@@ -9384,55 +9383,55 @@
         <v>0.46</v>
       </c>
       <c r="AE23">
-        <f t="shared" ref="AE23:AQ23" si="20">AD23</f>
+        <f t="shared" ref="AE23:AQ23" si="18">AD23</f>
         <v>0.46</v>
       </c>
       <c r="AF23">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>0.46</v>
       </c>
       <c r="AG23">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>0.46</v>
       </c>
       <c r="AH23">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>0.46</v>
       </c>
       <c r="AI23">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>0.46</v>
       </c>
       <c r="AJ23">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>0.46</v>
       </c>
       <c r="AK23">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>0.46</v>
       </c>
       <c r="AL23">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>0.46</v>
       </c>
       <c r="AM23">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>0.46</v>
       </c>
       <c r="AN23">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>0.46</v>
       </c>
       <c r="AO23">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>0.46</v>
       </c>
       <c r="AP23">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>0.46</v>
       </c>
       <c r="AQ23">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>0.46</v>
       </c>
       <c r="AR23">
@@ -9444,32 +9443,32 @@
         <v>0.46</v>
       </c>
       <c r="AT23">
-        <f t="shared" si="15"/>
+        <f t="shared" si="12"/>
         <v>0.46</v>
       </c>
       <c r="AU23">
-        <f t="shared" si="15"/>
+        <f t="shared" si="12"/>
         <v>0.46</v>
       </c>
     </row>
     <row r="24" spans="1:47" x14ac:dyDescent="0.45">
       <c r="A24">
-        <f t="shared" si="3"/>
+        <f>A23+1</f>
         <v>2040</v>
       </c>
       <c r="B24">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v>76</v>
       </c>
       <c r="C24">
-        <f t="shared" si="1"/>
+        <f>B24/100</f>
         <v>0.76</v>
       </c>
       <c r="L24" t="s">
         <v>23</v>
       </c>
       <c r="M24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="2"/>
         <v>0.3</v>
       </c>
       <c r="N24">
@@ -9489,137 +9488,137 @@
         <v>0.3</v>
       </c>
       <c r="R24">
-        <f t="shared" ref="R24:AU24" si="21">Q24</f>
+        <f t="shared" ref="R24:AU24" si="19">Q24</f>
         <v>0.3</v>
       </c>
       <c r="S24">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0.3</v>
       </c>
       <c r="T24">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0.3</v>
       </c>
       <c r="U24">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0.3</v>
       </c>
       <c r="V24">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0.3</v>
       </c>
       <c r="W24">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0.3</v>
       </c>
       <c r="X24">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0.3</v>
       </c>
       <c r="Y24">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0.3</v>
       </c>
       <c r="Z24">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0.3</v>
       </c>
       <c r="AA24">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0.3</v>
       </c>
       <c r="AB24">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0.3</v>
       </c>
       <c r="AC24">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0.3</v>
       </c>
       <c r="AD24">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0.3</v>
       </c>
       <c r="AE24">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0.3</v>
       </c>
       <c r="AF24">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0.3</v>
       </c>
       <c r="AG24">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0.3</v>
       </c>
       <c r="AH24">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0.3</v>
       </c>
       <c r="AI24">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0.3</v>
       </c>
       <c r="AJ24">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0.3</v>
       </c>
       <c r="AK24">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0.3</v>
       </c>
       <c r="AL24">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0.3</v>
       </c>
       <c r="AM24">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0.3</v>
       </c>
       <c r="AN24">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0.3</v>
       </c>
       <c r="AO24">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0.3</v>
       </c>
       <c r="AP24">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0.3</v>
       </c>
       <c r="AQ24">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0.3</v>
       </c>
       <c r="AR24">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0.3</v>
       </c>
       <c r="AS24">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0.3</v>
       </c>
       <c r="AT24">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0.3</v>
       </c>
       <c r="AU24">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0.3</v>
       </c>
     </row>
     <row r="25" spans="1:47" x14ac:dyDescent="0.45">
       <c r="A25">
-        <f t="shared" si="3"/>
+        <f>A24+1</f>
         <v>2041</v>
       </c>
       <c r="B25">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v>76</v>
       </c>
       <c r="C25">
-        <f t="shared" si="1"/>
+        <f>B25/100</f>
         <v>0.76</v>
       </c>
       <c r="L25" t="s">
@@ -9634,149 +9633,149 @@
         <v>0.22689835106537268</v>
       </c>
       <c r="O25">
-        <f t="shared" ref="O25:AU26" si="22">N25</f>
+        <f t="shared" ref="O25:AU26" si="20">N25</f>
         <v>0.22689835106537268</v>
       </c>
       <c r="P25">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.22689835106537268</v>
       </c>
       <c r="Q25">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.22689835106537268</v>
       </c>
       <c r="R25">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.22689835106537268</v>
       </c>
       <c r="S25">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.22689835106537268</v>
       </c>
       <c r="T25">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.22689835106537268</v>
       </c>
       <c r="U25">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.22689835106537268</v>
       </c>
       <c r="V25">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.22689835106537268</v>
       </c>
       <c r="W25">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.22689835106537268</v>
       </c>
       <c r="X25">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.22689835106537268</v>
       </c>
       <c r="Y25">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.22689835106537268</v>
       </c>
       <c r="Z25">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.22689835106537268</v>
       </c>
       <c r="AA25">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.22689835106537268</v>
       </c>
       <c r="AB25">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.22689835106537268</v>
       </c>
       <c r="AC25">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.22689835106537268</v>
       </c>
       <c r="AD25">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.22689835106537268</v>
       </c>
       <c r="AE25">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.22689835106537268</v>
       </c>
       <c r="AF25">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.22689835106537268</v>
       </c>
       <c r="AG25">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.22689835106537268</v>
       </c>
       <c r="AH25">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.22689835106537268</v>
       </c>
       <c r="AI25">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.22689835106537268</v>
       </c>
       <c r="AJ25">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.22689835106537268</v>
       </c>
       <c r="AK25">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.22689835106537268</v>
       </c>
       <c r="AL25">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.22689835106537268</v>
       </c>
       <c r="AM25">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.22689835106537268</v>
       </c>
       <c r="AN25">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.22689835106537268</v>
       </c>
       <c r="AO25">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.22689835106537268</v>
       </c>
       <c r="AP25">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.22689835106537268</v>
       </c>
       <c r="AQ25">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.22689835106537268</v>
       </c>
       <c r="AR25">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.22689835106537268</v>
       </c>
       <c r="AS25">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.22689835106537268</v>
       </c>
       <c r="AT25">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.22689835106537268</v>
       </c>
       <c r="AU25">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.22689835106537268</v>
       </c>
     </row>
     <row r="26" spans="1:47" x14ac:dyDescent="0.45">
       <c r="A26">
-        <f t="shared" si="3"/>
+        <f>A25+1</f>
         <v>2042</v>
       </c>
       <c r="B26">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v>76</v>
       </c>
       <c r="C26">
-        <f t="shared" si="1"/>
+        <f>B26/100</f>
         <v>0.76</v>
       </c>
       <c r="L26" t="s">
@@ -9791,149 +9790,149 @@
         <v>0.14120000000000002</v>
       </c>
       <c r="O26">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.14120000000000002</v>
       </c>
       <c r="P26">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.14120000000000002</v>
       </c>
       <c r="Q26">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.14120000000000002</v>
       </c>
       <c r="R26">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.14120000000000002</v>
       </c>
       <c r="S26">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.14120000000000002</v>
       </c>
       <c r="T26">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.14120000000000002</v>
       </c>
       <c r="U26">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.14120000000000002</v>
       </c>
       <c r="V26">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.14120000000000002</v>
       </c>
       <c r="W26">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.14120000000000002</v>
       </c>
       <c r="X26">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.14120000000000002</v>
       </c>
       <c r="Y26">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.14120000000000002</v>
       </c>
       <c r="Z26">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.14120000000000002</v>
       </c>
       <c r="AA26">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.14120000000000002</v>
       </c>
       <c r="AB26">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.14120000000000002</v>
       </c>
       <c r="AC26">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.14120000000000002</v>
       </c>
       <c r="AD26">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.14120000000000002</v>
       </c>
       <c r="AE26">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.14120000000000002</v>
       </c>
       <c r="AF26">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.14120000000000002</v>
       </c>
       <c r="AG26">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.14120000000000002</v>
       </c>
       <c r="AH26">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.14120000000000002</v>
       </c>
       <c r="AI26">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.14120000000000002</v>
       </c>
       <c r="AJ26">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.14120000000000002</v>
       </c>
       <c r="AK26">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.14120000000000002</v>
       </c>
       <c r="AL26">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.14120000000000002</v>
       </c>
       <c r="AM26">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.14120000000000002</v>
       </c>
       <c r="AN26">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.14120000000000002</v>
       </c>
       <c r="AO26">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.14120000000000002</v>
       </c>
       <c r="AP26">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.14120000000000002</v>
       </c>
       <c r="AQ26">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.14120000000000002</v>
       </c>
       <c r="AR26">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.14120000000000002</v>
       </c>
       <c r="AS26">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.14120000000000002</v>
       </c>
       <c r="AT26">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.14120000000000002</v>
       </c>
       <c r="AU26">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>0.14120000000000002</v>
       </c>
     </row>
     <row r="27" spans="1:47" x14ac:dyDescent="0.45">
       <c r="A27">
-        <f t="shared" si="3"/>
+        <f>A26+1</f>
         <v>2043</v>
       </c>
       <c r="B27">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v>76</v>
       </c>
       <c r="C27">
-        <f t="shared" si="1"/>
+        <f>B27/100</f>
         <v>0.76</v>
       </c>
       <c r="L27" t="s">
@@ -9948,149 +9947,149 @@
         <v>0.11790000000000003</v>
       </c>
       <c r="O27">
-        <f t="shared" ref="O27:AU27" si="23">N27</f>
+        <f t="shared" ref="O27:AU27" si="21">N27</f>
         <v>0.11790000000000003</v>
       </c>
       <c r="P27">
-        <f t="shared" si="23"/>
+        <f t="shared" si="21"/>
         <v>0.11790000000000003</v>
       </c>
       <c r="Q27">
-        <f t="shared" si="23"/>
+        <f t="shared" si="21"/>
         <v>0.11790000000000003</v>
       </c>
       <c r="R27">
-        <f t="shared" si="23"/>
+        <f t="shared" si="21"/>
         <v>0.11790000000000003</v>
       </c>
       <c r="S27">
-        <f t="shared" si="23"/>
+        <f t="shared" si="21"/>
         <v>0.11790000000000003</v>
       </c>
       <c r="T27">
-        <f t="shared" si="23"/>
+        <f t="shared" si="21"/>
         <v>0.11790000000000003</v>
       </c>
       <c r="U27">
-        <f t="shared" si="23"/>
+        <f t="shared" si="21"/>
         <v>0.11790000000000003</v>
       </c>
       <c r="V27">
-        <f t="shared" si="23"/>
+        <f t="shared" si="21"/>
         <v>0.11790000000000003</v>
       </c>
       <c r="W27">
-        <f t="shared" si="23"/>
+        <f t="shared" si="21"/>
         <v>0.11790000000000003</v>
       </c>
       <c r="X27">
-        <f t="shared" si="23"/>
+        <f t="shared" si="21"/>
         <v>0.11790000000000003</v>
       </c>
       <c r="Y27">
-        <f t="shared" si="23"/>
+        <f t="shared" si="21"/>
         <v>0.11790000000000003</v>
       </c>
       <c r="Z27">
-        <f t="shared" si="23"/>
+        <f t="shared" si="21"/>
         <v>0.11790000000000003</v>
       </c>
       <c r="AA27">
-        <f t="shared" si="23"/>
+        <f t="shared" si="21"/>
         <v>0.11790000000000003</v>
       </c>
       <c r="AB27">
-        <f t="shared" si="23"/>
+        <f t="shared" si="21"/>
         <v>0.11790000000000003</v>
       </c>
       <c r="AC27">
-        <f t="shared" si="23"/>
+        <f t="shared" si="21"/>
         <v>0.11790000000000003</v>
       </c>
       <c r="AD27">
-        <f t="shared" si="23"/>
+        <f t="shared" si="21"/>
         <v>0.11790000000000003</v>
       </c>
       <c r="AE27">
-        <f t="shared" si="23"/>
+        <f t="shared" si="21"/>
         <v>0.11790000000000003</v>
       </c>
       <c r="AF27">
-        <f t="shared" si="23"/>
+        <f t="shared" si="21"/>
         <v>0.11790000000000003</v>
       </c>
       <c r="AG27">
-        <f t="shared" si="23"/>
+        <f t="shared" si="21"/>
         <v>0.11790000000000003</v>
       </c>
       <c r="AH27">
-        <f t="shared" si="23"/>
+        <f t="shared" si="21"/>
         <v>0.11790000000000003</v>
       </c>
       <c r="AI27">
-        <f t="shared" si="23"/>
+        <f t="shared" si="21"/>
         <v>0.11790000000000003</v>
       </c>
       <c r="AJ27">
-        <f t="shared" si="23"/>
+        <f t="shared" si="21"/>
         <v>0.11790000000000003</v>
       </c>
       <c r="AK27">
-        <f t="shared" si="23"/>
+        <f t="shared" si="21"/>
         <v>0.11790000000000003</v>
       </c>
       <c r="AL27">
-        <f t="shared" si="23"/>
+        <f t="shared" si="21"/>
         <v>0.11790000000000003</v>
       </c>
       <c r="AM27">
-        <f t="shared" si="23"/>
+        <f t="shared" si="21"/>
         <v>0.11790000000000003</v>
       </c>
       <c r="AN27">
-        <f t="shared" si="23"/>
+        <f t="shared" si="21"/>
         <v>0.11790000000000003</v>
       </c>
       <c r="AO27">
-        <f t="shared" si="23"/>
+        <f t="shared" si="21"/>
         <v>0.11790000000000003</v>
       </c>
       <c r="AP27">
-        <f t="shared" si="23"/>
+        <f t="shared" si="21"/>
         <v>0.11790000000000003</v>
       </c>
       <c r="AQ27">
-        <f t="shared" si="23"/>
+        <f t="shared" si="21"/>
         <v>0.11790000000000003</v>
       </c>
       <c r="AR27">
-        <f t="shared" si="23"/>
+        <f t="shared" si="21"/>
         <v>0.11790000000000003</v>
       </c>
       <c r="AS27">
-        <f t="shared" si="23"/>
+        <f t="shared" si="21"/>
         <v>0.11790000000000003</v>
       </c>
       <c r="AT27">
-        <f t="shared" si="23"/>
+        <f t="shared" si="21"/>
         <v>0.11790000000000003</v>
       </c>
       <c r="AU27">
-        <f t="shared" si="23"/>
+        <f t="shared" si="21"/>
         <v>0.11790000000000003</v>
       </c>
     </row>
     <row r="28" spans="1:47" x14ac:dyDescent="0.45">
       <c r="A28">
-        <f t="shared" si="3"/>
+        <f>A27+1</f>
         <v>2044</v>
       </c>
       <c r="B28">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v>76</v>
       </c>
       <c r="C28">
-        <f t="shared" si="1"/>
+        <f>B28/100</f>
         <v>0.76</v>
       </c>
       <c r="L28" t="s">
@@ -10117,47 +10116,47 @@
         <v>0.58338461538461317</v>
       </c>
       <c r="R28">
-        <f t="shared" ref="R28:AB28" si="24">FORECAST(R16,$Q$14:$R$14,$Q$2:$R$2)</f>
+        <f t="shared" ref="R28:AB28" si="22">FORECAST(R16,$Q$14:$R$14,$Q$2:$R$2)</f>
         <v>0.59726923076922844</v>
       </c>
       <c r="S28">
-        <f t="shared" si="24"/>
+        <f t="shared" si="22"/>
         <v>0.61115384615384372</v>
       </c>
       <c r="T28">
-        <f t="shared" si="24"/>
+        <f t="shared" si="22"/>
         <v>0.62503846153845899</v>
       </c>
       <c r="U28">
-        <f t="shared" si="24"/>
+        <f t="shared" si="22"/>
         <v>0.63892307692307426</v>
       </c>
       <c r="V28">
-        <f t="shared" si="24"/>
+        <f t="shared" si="22"/>
         <v>0.65280769230768954</v>
       </c>
       <c r="W28">
-        <f t="shared" si="24"/>
+        <f t="shared" si="22"/>
         <v>0.66669230769230481</v>
       </c>
       <c r="X28">
-        <f t="shared" si="24"/>
+        <f t="shared" si="22"/>
         <v>0.68057692307692008</v>
       </c>
       <c r="Y28">
-        <f t="shared" si="24"/>
+        <f t="shared" si="22"/>
         <v>0.69446153846153535</v>
       </c>
       <c r="Z28">
-        <f t="shared" si="24"/>
+        <f t="shared" si="22"/>
         <v>0.70834615384615063</v>
       </c>
       <c r="AA28">
-        <f t="shared" si="24"/>
+        <f t="shared" si="22"/>
         <v>0.7222307692307659</v>
       </c>
       <c r="AB28">
-        <f t="shared" si="24"/>
+        <f t="shared" si="22"/>
         <v>0.73611538461538117</v>
       </c>
       <c r="AC28">
@@ -10169,55 +10168,55 @@
         <v>0.7506666666666667</v>
       </c>
       <c r="AE28">
-        <f t="shared" ref="AE28:AQ28" si="25">FORECAST(AE16,$R$14:$S$14,$R$2:$S$2)</f>
+        <f t="shared" ref="AE28:AQ28" si="23">FORECAST(AE16,$R$14:$S$14,$R$2:$S$2)</f>
         <v>0.7513333333333333</v>
       </c>
       <c r="AF28">
-        <f t="shared" si="25"/>
+        <f t="shared" si="23"/>
         <v>0.75200000000000011</v>
       </c>
       <c r="AG28">
-        <f t="shared" si="25"/>
+        <f t="shared" si="23"/>
         <v>0.75266666666666671</v>
       </c>
       <c r="AH28">
-        <f t="shared" si="25"/>
+        <f t="shared" si="23"/>
         <v>0.7533333333333333</v>
       </c>
       <c r="AI28">
-        <f t="shared" si="25"/>
+        <f t="shared" si="23"/>
         <v>0.75400000000000011</v>
       </c>
       <c r="AJ28">
-        <f t="shared" si="25"/>
+        <f t="shared" si="23"/>
         <v>0.75466666666666671</v>
       </c>
       <c r="AK28">
-        <f t="shared" si="25"/>
+        <f t="shared" si="23"/>
         <v>0.7553333333333333</v>
       </c>
       <c r="AL28">
-        <f t="shared" si="25"/>
+        <f t="shared" si="23"/>
         <v>0.75600000000000012</v>
       </c>
       <c r="AM28">
-        <f t="shared" si="25"/>
+        <f t="shared" si="23"/>
         <v>0.75666666666666671</v>
       </c>
       <c r="AN28">
-        <f t="shared" si="25"/>
+        <f t="shared" si="23"/>
         <v>0.7573333333333333</v>
       </c>
       <c r="AO28">
-        <f t="shared" si="25"/>
+        <f t="shared" si="23"/>
         <v>0.75800000000000012</v>
       </c>
       <c r="AP28">
-        <f t="shared" si="25"/>
+        <f t="shared" si="23"/>
         <v>0.75866666666666671</v>
       </c>
       <c r="AQ28">
-        <f t="shared" si="25"/>
+        <f t="shared" si="23"/>
         <v>0.7593333333333333</v>
       </c>
       <c r="AR28">
@@ -10229,25 +10228,25 @@
         <v>0.76</v>
       </c>
       <c r="AT28">
-        <f t="shared" ref="AT28:AU28" si="26">AS28</f>
+        <f t="shared" ref="AT28:AU28" si="24">AS28</f>
         <v>0.76</v>
       </c>
       <c r="AU28">
-        <f t="shared" si="26"/>
+        <f t="shared" si="24"/>
         <v>0.76</v>
       </c>
     </row>
     <row r="29" spans="1:47" x14ac:dyDescent="0.45">
       <c r="A29">
-        <f t="shared" si="3"/>
+        <f>A28+1</f>
         <v>2045</v>
       </c>
       <c r="B29">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v>76</v>
       </c>
       <c r="C29">
-        <f t="shared" si="1"/>
+        <f>B29/100</f>
         <v>0.76</v>
       </c>
       <c r="L29" t="s">
@@ -10274,47 +10273,47 @@
         <v>0.36</v>
       </c>
       <c r="R29">
-        <f t="shared" ref="R29:AB29" si="27">Q29</f>
+        <f t="shared" ref="R29:AB29" si="25">Q29</f>
         <v>0.36</v>
       </c>
       <c r="S29">
-        <f t="shared" si="27"/>
+        <f t="shared" si="25"/>
         <v>0.36</v>
       </c>
       <c r="T29">
-        <f t="shared" si="27"/>
+        <f t="shared" si="25"/>
         <v>0.36</v>
       </c>
       <c r="U29">
-        <f t="shared" si="27"/>
+        <f t="shared" si="25"/>
         <v>0.36</v>
       </c>
       <c r="V29">
-        <f t="shared" si="27"/>
+        <f t="shared" si="25"/>
         <v>0.36</v>
       </c>
       <c r="W29">
-        <f t="shared" si="27"/>
+        <f t="shared" si="25"/>
         <v>0.36</v>
       </c>
       <c r="X29">
-        <f t="shared" si="27"/>
+        <f t="shared" si="25"/>
         <v>0.36</v>
       </c>
       <c r="Y29">
-        <f t="shared" si="27"/>
+        <f t="shared" si="25"/>
         <v>0.36</v>
       </c>
       <c r="Z29">
-        <f t="shared" si="27"/>
+        <f t="shared" si="25"/>
         <v>0.36</v>
       </c>
       <c r="AA29">
-        <f t="shared" si="27"/>
+        <f t="shared" si="25"/>
         <v>0.36</v>
       </c>
       <c r="AB29">
-        <f t="shared" si="27"/>
+        <f t="shared" si="25"/>
         <v>0.36</v>
       </c>
       <c r="AC29">
@@ -10326,55 +10325,55 @@
         <v>0.3620000000000001</v>
       </c>
       <c r="AE29">
-        <f t="shared" ref="AE29:AQ29" si="28">FORECAST(AE16,$R$11:$S$11,$R$2:$S$2)</f>
+        <f t="shared" ref="AE29:AQ29" si="26">FORECAST(AE16,$R$11:$S$11,$R$2:$S$2)</f>
         <v>0.36399999999999988</v>
       </c>
       <c r="AF29">
-        <f t="shared" si="28"/>
+        <f t="shared" si="26"/>
         <v>0.36600000000000055</v>
       </c>
       <c r="AG29">
-        <f t="shared" si="28"/>
+        <f t="shared" si="26"/>
         <v>0.36800000000000033</v>
       </c>
       <c r="AH29">
-        <f t="shared" si="28"/>
+        <f t="shared" si="26"/>
         <v>0.37000000000000011</v>
       </c>
       <c r="AI29">
-        <f t="shared" si="28"/>
+        <f t="shared" si="26"/>
         <v>0.37200000000000077</v>
       </c>
       <c r="AJ29">
-        <f t="shared" si="28"/>
+        <f t="shared" si="26"/>
         <v>0.37400000000000055</v>
       </c>
       <c r="AK29">
-        <f t="shared" si="28"/>
+        <f t="shared" si="26"/>
         <v>0.37600000000000033</v>
       </c>
       <c r="AL29">
-        <f t="shared" si="28"/>
+        <f t="shared" si="26"/>
         <v>0.37800000000000011</v>
       </c>
       <c r="AM29">
-        <f t="shared" si="28"/>
+        <f t="shared" si="26"/>
         <v>0.37999999999999989</v>
       </c>
       <c r="AN29">
-        <f t="shared" si="28"/>
+        <f t="shared" si="26"/>
         <v>0.38200000000000056</v>
       </c>
       <c r="AO29">
-        <f t="shared" si="28"/>
+        <f t="shared" si="26"/>
         <v>0.38400000000000034</v>
       </c>
       <c r="AP29">
-        <f t="shared" si="28"/>
+        <f t="shared" si="26"/>
         <v>0.38600000000000012</v>
       </c>
       <c r="AQ29">
-        <f t="shared" si="28"/>
+        <f t="shared" si="26"/>
         <v>0.38800000000000079</v>
       </c>
       <c r="AR29">
@@ -10386,82 +10385,82 @@
         <v>0.39</v>
       </c>
       <c r="AT29">
-        <f t="shared" ref="AT29:AU29" si="29">AS29</f>
+        <f t="shared" ref="AT29:AU29" si="27">AS29</f>
         <v>0.39</v>
       </c>
       <c r="AU29">
-        <f t="shared" si="29"/>
+        <f t="shared" si="27"/>
         <v>0.39</v>
       </c>
     </row>
     <row r="30" spans="1:47" x14ac:dyDescent="0.45">
       <c r="A30">
-        <f t="shared" si="3"/>
+        <f>A29+1</f>
         <v>2046</v>
       </c>
       <c r="B30">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v>76</v>
       </c>
       <c r="C30">
-        <f t="shared" si="1"/>
+        <f>B30/100</f>
         <v>0.76</v>
       </c>
     </row>
     <row r="31" spans="1:47" x14ac:dyDescent="0.45">
       <c r="A31">
-        <f t="shared" si="3"/>
+        <f>A30+1</f>
         <v>2047</v>
       </c>
       <c r="B31">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v>76</v>
       </c>
       <c r="C31">
-        <f t="shared" si="1"/>
+        <f>B31/100</f>
         <v>0.76</v>
       </c>
       <c r="AS31" s="1"/>
     </row>
     <row r="32" spans="1:47" x14ac:dyDescent="0.45">
       <c r="A32">
-        <f t="shared" si="3"/>
+        <f>A31+1</f>
         <v>2048</v>
       </c>
       <c r="B32">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v>76</v>
       </c>
       <c r="C32">
-        <f t="shared" si="1"/>
+        <f>B32/100</f>
         <v>0.76</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A33">
-        <f t="shared" si="3"/>
+        <f>A32+1</f>
         <v>2049</v>
       </c>
       <c r="B33">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v>76</v>
       </c>
       <c r="C33">
-        <f t="shared" si="1"/>
+        <f>B33/100</f>
         <v>0.76</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A34">
-        <f t="shared" si="3"/>
+        <f>A33+1</f>
         <v>2050</v>
       </c>
       <c r="B34">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v>76</v>
       </c>
       <c r="C34">
-        <f t="shared" si="1"/>
+        <f>B34/100</f>
         <v>0.76</v>
       </c>
     </row>
@@ -10484,7 +10483,7 @@
   <dimension ref="A1:AJ17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:AJ10"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -16232,71 +16231,71 @@
       </c>
       <c r="B7" s="7">
         <f>Calculations!M22</f>
-        <v>0.24</v>
+        <v>0.21</v>
       </c>
       <c r="C7" s="7">
         <f>Calculations!N22</f>
-        <v>0.24</v>
+        <v>0.21</v>
       </c>
       <c r="D7" s="7">
         <f>Calculations!O22</f>
-        <v>0.24</v>
+        <v>0.21</v>
       </c>
       <c r="E7" s="7">
         <f>Calculations!P22</f>
-        <v>0.24</v>
+        <v>0.21</v>
       </c>
       <c r="F7" s="7">
         <f>Calculations!Q22</f>
-        <v>0.24</v>
+        <v>0.21230769230769209</v>
       </c>
       <c r="G7" s="7">
         <f>Calculations!R22</f>
-        <v>0.24</v>
+        <v>0.21461538461538421</v>
       </c>
       <c r="H7" s="7">
         <f>Calculations!S22</f>
-        <v>0.24</v>
+        <v>0.21692307692307722</v>
       </c>
       <c r="I7" s="7">
         <f>Calculations!T22</f>
-        <v>0.24</v>
+        <v>0.21923076923076934</v>
       </c>
       <c r="J7" s="7">
         <f>Calculations!U22</f>
-        <v>0.24</v>
+        <v>0.22153846153846146</v>
       </c>
       <c r="K7" s="7">
         <f>Calculations!V22</f>
-        <v>0.24</v>
+        <v>0.22384615384615358</v>
       </c>
       <c r="L7" s="7">
         <f>Calculations!W22</f>
-        <v>0.24</v>
+        <v>0.22615384615384571</v>
       </c>
       <c r="M7" s="7">
         <f>Calculations!X22</f>
-        <v>0.24</v>
+        <v>0.22846153846153872</v>
       </c>
       <c r="N7" s="7">
         <f>Calculations!Y22</f>
-        <v>0.24</v>
+        <v>0.23076923076923084</v>
       </c>
       <c r="O7" s="7">
         <f>Calculations!Z22</f>
-        <v>0.24</v>
+        <v>0.23307692307692296</v>
       </c>
       <c r="P7" s="7">
         <f>Calculations!AA22</f>
-        <v>0.24</v>
+        <v>0.23538461538461508</v>
       </c>
       <c r="Q7" s="7">
         <f>Calculations!AB22</f>
-        <v>0.24</v>
+        <v>0.2376923076923072</v>
       </c>
       <c r="R7" s="7">
         <f>Calculations!AC22</f>
-        <v>0.24</v>
+        <v>0.24000000000000021</v>
       </c>
       <c r="S7" s="7">
         <f>Calculations!AD22</f>

</xml_diff>